<commit_message>
updated app.py, resolved error
</commit_message>
<xml_diff>
--- a/updated_data.xlsx
+++ b/updated_data.xlsx
@@ -522,32 +522,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>40489544</t>
+          <t>40521480</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Mr ABU MAJED</t>
+          <t>Mr DHAIFALLAH ALENEZI</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>009661</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Plat Xtra HD 2013</t>
+          <t>Premier 2014</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>03/03/2016</t>
+          <t>20/09/2014</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>25/02/2016</t>
+          <t>11/01/2015</t>
         </is>
       </c>
     </row>
@@ -560,32 +560,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20117454</t>
+          <t>40521480</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mr SULTAN HAMMAD ALMAHDY</t>
+          <t>Mr DHAIFALLAH ALENEZI</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>00966558491663</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>Premier 2014</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>26/07/2017</t>
+          <t>20/09/2014</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>30/07/2016</t>
+          <t>11/01/2015</t>
         </is>
       </c>
     </row>

</xml_diff>